<commit_message>
fixing errors in fastq file names for 08.27.20 sheet
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_J.PLAGGENBERG_08.27.20.xlsx
+++ b/fastqFiles/fastq_J.PLAGGENBERG_08.27.20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8678D6-5DF7-4C44-9138-566EB33574E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0214CAE4-BDBA-C746-BDCC-43BE4D2895B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="19960" windowHeight="19840" xr2:uid="{C08B94BE-58C1-0249-822A-140ACB8B1927}"/>
+    <workbookView xWindow="10180" yWindow="460" windowWidth="27080" windowHeight="19840" xr2:uid="{C08B94BE-58C1-0249-822A-140ACB8B1927}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,24 +80,6 @@
     <t>fullRNASeq</t>
   </si>
   <si>
-    <t>Brent_Large/Brent_R5_1_GTAC_3_SIC_Index2_06_ATGACAG_GACCTTGT_S20_R1_001.fastq.gz:</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_2_GTAC_4_SIC_Index2_06_CACCTCC_GACCTTGT_S21_R1_001.fastq.gz:</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_3_GTAC_6_SIC_Index2_06_TACTCTA_GACCTTGT_S22_R1_001.fastq.gz:</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R5_4_GTAC_7_SIC_Index2_06_AGACTGA_GACCTTGT_S71_R1_001.fastq.gz:</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R5_5_GTAC_8_SIC_Index2_06_CTTGGAA_GACCTTGT_S72_R1_001.fastq.gz:</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_6_GTAC_9_SIC_Index2_06_CCGATTA_GACCTTGT_S23_R1_001.fastq.gz:</t>
-  </si>
-  <si>
     <t>Brent_Small/Brent_R5_7_GTAC_11_SIC_Index2_06_CCATCAT_GACCTTGT_S73_R1_001.fastq.gz</t>
   </si>
   <si>
@@ -107,99 +89,6 @@
     <t>Brent_Large/Brent_R5_9_GTAC_14_SIC_Index2_06_TTTAACT_GACCTTGT_S25_R1_001.fastq.gz</t>
   </si>
   <si>
-    <t>Brent_Large/Brent_R5_10_GTAC_15_SIC_Index2_06_GGTCCTC_GACCTTGT_S26_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_11_GTAC_16_SIC_Index2_06_CGGTGGC_GACCTTGT_S27_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R5_12_GTAC_17_SIC_Index2_06_ACTGTCG_GACCTTGT_S74_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_13_GTAC_18_SIC_Index2_06_GTATTTG_GACCTTGT_S28_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_14_GTAC_19_SIC_Index2_06_GAGTACG_GACCTTGT_S29_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_15_GTAC_20_SIC_Index2_06_ACAGATA_GACCTTGT_S30_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_16_GTAC_21_SIC_Index2_06_CTCAATG_GACCTTGT_S31_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_17_GTAC_22_SIC_Index2_06_AAATGCA_GACCTTGT_S32_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_18_GTAC_23_SIC_Index2_06_ACGCGGG_GACCTTGT_S33_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_19_GTAC_24_SIC_Index2_06_GGAGTCC_GACCTTGT_S34_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_20_GTAC_25_SIC_Index2_06_CGTCGCT_GACCTTGT_S35_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_21_GTAC_26_SIC_Index2_06_TCAACTG_GACCTTGT_S36_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R5_22_GTAC_27_SIC_Index2_06_TGTTTGT_GACCTTGT_S75_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R5_23_GTAC_28_SIC_Index2_06_TACATGG_GACCTTGT_S76_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_24_GTAC_29_SIC_Index2_06_GTTCTCA_GACCTTGT_S37_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_25_GTAC_30_SIC_Index2_06_CTGGTGG_GACCTTGT_S38_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_26_GTAC_31_SIC_Index2_06_TGCCCAT_GACCTTGT_S39_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_27_GTAC_32_SIC_Index2_06_AAACCTT_GACCTTGT_S40_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_28_GTAC_33_SIC_Index2_06_ACCATAC_GACCTTGT_S41_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_29_GTAC_34_SIC_Index2_06_AATACGC_GACCTTGT_S42_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_30_GTAC_35_SIC_Index2_06_CGCTACA_GACCTTGT_S43_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R5_31_GTAC_36_SIC_Index2_06_TGGCATA_GACCTTGT_S77_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_32_GTAC_37_SIC_Index2_06_TTTTGTC_GACCTTGT_S44_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_33_GTAC_38_SIC_Index2_06_ACCCACT_GACCTTGT_S45_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R5_34_GTAC_39_SIC_Index2_06_CCGGACC_GACCTTGT_S78_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R5_35_GTAC_40_SIC_Index2_06_GTACGGC_GACCTTGT_S79_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R5_36_GTAC_41_SIC_Index2_06_TTGCCCC_GACCTTGT_S80_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_37_GTAC_42_SIC_Index2_06_ACTCCAA_GACCTTGT_S46_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R5_38_GTAC_43_SIC_Index2_06_TGTGCCA_GACCTTGT_S81_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_39_GTAC_44_SIC_Index2_06_AACGGAG_GACCTTGT_S47_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R5_40_GTAC_45_SIC_Index2_06_GATAGTT_GACCTTGT_S48_R1_001.fastq.g</t>
-  </si>
-  <si>
     <t>06.18.20</t>
   </si>
   <si>
@@ -209,127 +98,238 @@
     <t>07.06.20</t>
   </si>
   <si>
-    <t>Brent_Large/Brent_R1_1_GTAC_21_SIC_Index2_08_CTCAATG_AAGCACGT_S2_R1_001.fastq.gz:</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_2_GTAC_22_SIC_Index2_08_AAATGCA_AAGCACGT_S3_R1_001.fastq.gz:</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_3_GTAC_23_SIC_Index2_08_ACGCGGG_AAGCACGT_S4_R1_001.fastq.gz:</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_4_GTAC_24_SIC_Index2_08_GGAGTCC_AAGCACGT_S5_R1_001.fastq.gz:</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_5_GTAC_25_SIC_Index2_08_CGTCGCT_AAGCACGT_S6_R1_001.fastq.gz:</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_6_GTAC_26_SIC_Index2_08_TCAACTG_AAGCACGT_S7_R1_001.fastq.gz:</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_7_GTAC_27_SIC_Index2_08_TGTTTGT_AAGCACGT_S8_R1_001.fastq.gz:</t>
-  </si>
-  <si>
     <t>Brent_Small/Brent_R1_8_GTAC_28_SIC_Index2_08_TACATGG_AAGCACGT_S49_R1_001.fastq.gz</t>
   </si>
   <si>
     <t>Brent_Small/Brent_R1_9_GTAC_29_SIC_Index2_08_GTTCTCA_AAGCACGT_S50_R1_001.fastq.gz</t>
   </si>
   <si>
-    <t>Brent_Small/Brent_R1_10_GTAC_30_SIC_Index2_08_CTGGTGG_AAGCACGT_S51_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_11_GTAC_31_SIC_Index2_08_TGCCCAT_AAGCACGT_S52_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_12_GTAC_32_SIC_Index2_08_AAACCTT_AAGCACGT_S53_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_13_GTAC_33_SIC_Index2_08_ACCATAC_AAGCACGT_S54_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_14_GTAC_34_SIC_Index2_08_AATACGC_AAGCACGT_S55_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_15_GTAC_35_SIC_Index2_08_CGCTACA_AAGCACGT_S56_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_16_GTAC_36_SIC_Index2_08_TGGCATA_AAGCACGT_S57_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_17_GTAC_37_SIC_Index2_08_TTTTGTC_AAGCACGT_S58_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_18_GTAC_38_SIC_Index2_08_ACCCACT_AAGCACGT_S59_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_19_GTAC_39_SIC_Index2_08_CCGGACC_AAGCACGT_S60_R1_001.fastq.g</t>
-  </si>
-  <si>
     <t>Brent_Large/Brent_R1_20_GTAC_40_SIC_Index2_08_GTACGGC_AAGCACGT_S9_R1_001.fastq.gz</t>
   </si>
   <si>
-    <t>Brent_Small/Brent_R1_21_GTAC_41_SIC_Index2_08_TTGCCCC_AAGCACGT_S61_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_22_GTAC_42_SIC_Index2_08_ACTCCAA_AAGCACGT_S10_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_23_GTAC_43_SIC_Index2_08_TGTGCCA_AAGCACGT_S11_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_24_GTAC_44_SIC_Index2_08_AACGGAG_AAGCACGT_S62_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_25_GTAC_45_SIC_Index2_08_GATAGTT_AAGCACGT_S63_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_26_GTAC_46_SIC_Index2_08_GGTGAAT_AAGCACGT_S64_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_27_GTAC_47_SIC_Index2_08_ATGTTCT_AAGCACGT_S12_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_28_GTAC_48_SIC_Index2_08_GTAAAAA_AAGCACGT_S13_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_29_GTAC_49_SIC_Index2_08_GTCTGAT_AAGCACGT_S14_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_30_GTAC_50_SIC_Index2_08_CAATATC_AAGCACGT_S15_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_31_GTAC_51_SIC_Index2_08_CTCCCGA_AAGCACGT_S65_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_32_GTAC_52_SIC_Index2_08_GCCGTTT_AAGCACGT_S66_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_33_GTAC_53_SIC_Index2_08_TAGGTAA_AAGCACGT_S67_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_34_GTAC_54_SIC_Index2_08_TCGAGAT_AAGCACGT_S16_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_35_GTAC_55_SIC_Index2_08_CATTTAG_AAGCACGT_S17_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_36_GTAC_56_SIC_Index2_08_TCCGGGA_AAGCACGT_S68_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_37_GTAC_57_SIC_Index2_08_CGAAAGT_AAGCACGT_S18_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_38_GTAC_58_SIC_Index2_08_GCCTCCC_AAGCACGT_S69_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Small/Brent_R1_39_GTAC_59_SIC_Index2_08_AGTTATG_AAGCACGT_S70_R1_001.fastq.g</t>
-  </si>
-  <si>
-    <t>Brent_Large/Brent_R1_40_GTAC_60_SIC_Index2_08_CTGCAAT_AAGCACGT_S19_R1_001.fastq.g</t>
-  </si>
-  <si>
     <t>08.03.20</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_1_GTAC_3_SIC_Index2_06_ATGACAG_GACCTTGT_S20_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_2_GTAC_4_SIC_Index2_06_CACCTCC_GACCTTGT_S21_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_3_GTAC_6_SIC_Index2_06_TACTCTA_GACCTTGT_S22_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R5_4_GTAC_7_SIC_Index2_06_AGACTGA_GACCTTGT_S71_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R5_5_GTAC_8_SIC_Index2_06_CTTGGAA_GACCTTGT_S72_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_6_GTAC_9_SIC_Index2_06_CCGATTA_GACCTTGT_S23_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_10_GTAC_15_SIC_Index2_06_GGTCCTC_GACCTTGT_S26_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_11_GTAC_16_SIC_Index2_06_CGGTGGC_GACCTTGT_S27_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R5_12_GTAC_17_SIC_Index2_06_ACTGTCG_GACCTTGT_S74_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_13_GTAC_18_SIC_Index2_06_GTATTTG_GACCTTGT_S28_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_14_GTAC_19_SIC_Index2_06_GAGTACG_GACCTTGT_S29_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_15_GTAC_20_SIC_Index2_06_ACAGATA_GACCTTGT_S30_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_16_GTAC_21_SIC_Index2_06_CTCAATG_GACCTTGT_S31_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_17_GTAC_22_SIC_Index2_06_AAATGCA_GACCTTGT_S32_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_18_GTAC_23_SIC_Index2_06_ACGCGGG_GACCTTGT_S33_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_19_GTAC_24_SIC_Index2_06_GGAGTCC_GACCTTGT_S34_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_20_GTAC_25_SIC_Index2_06_CGTCGCT_GACCTTGT_S35_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_21_GTAC_26_SIC_Index2_06_TCAACTG_GACCTTGT_S36_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R5_22_GTAC_27_SIC_Index2_06_TGTTTGT_GACCTTGT_S75_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R5_23_GTAC_28_SIC_Index2_06_TACATGG_GACCTTGT_S76_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_24_GTAC_29_SIC_Index2_06_GTTCTCA_GACCTTGT_S37_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_25_GTAC_30_SIC_Index2_06_CTGGTGG_GACCTTGT_S38_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_26_GTAC_31_SIC_Index2_06_TGCCCAT_GACCTTGT_S39_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_27_GTAC_32_SIC_Index2_06_AAACCTT_GACCTTGT_S40_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_28_GTAC_33_SIC_Index2_06_ACCATAC_GACCTTGT_S41_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_29_GTAC_34_SIC_Index2_06_AATACGC_GACCTTGT_S42_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_30_GTAC_35_SIC_Index2_06_CGCTACA_GACCTTGT_S43_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R5_31_GTAC_36_SIC_Index2_06_TGGCATA_GACCTTGT_S77_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_32_GTAC_37_SIC_Index2_06_TTTTGTC_GACCTTGT_S44_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_33_GTAC_38_SIC_Index2_06_ACCCACT_GACCTTGT_S45_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R5_34_GTAC_39_SIC_Index2_06_CCGGACC_GACCTTGT_S78_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R5_35_GTAC_40_SIC_Index2_06_GTACGGC_GACCTTGT_S79_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R5_36_GTAC_41_SIC_Index2_06_TTGCCCC_GACCTTGT_S80_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_37_GTAC_42_SIC_Index2_06_ACTCCAA_GACCTTGT_S46_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R5_38_GTAC_43_SIC_Index2_06_TGTGCCA_GACCTTGT_S81_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_39_GTAC_44_SIC_Index2_06_AACGGAG_GACCTTGT_S47_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R5_40_GTAC_45_SIC_Index2_06_GATAGTT_GACCTTGT_S48_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_1_GTAC_21_SIC_Index2_08_CTCAATG_AAGCACGT_S2_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_2_GTAC_22_SIC_Index2_08_AAATGCA_AAGCACGT_S3_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_3_GTAC_23_SIC_Index2_08_ACGCGGG_AAGCACGT_S4_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_4_GTAC_24_SIC_Index2_08_GGAGTCC_AAGCACGT_S5_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_5_GTAC_25_SIC_Index2_08_CGTCGCT_AAGCACGT_S6_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_6_GTAC_26_SIC_Index2_08_TCAACTG_AAGCACGT_S7_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_7_GTAC_27_SIC_Index2_08_TGTTTGT_AAGCACGT_S8_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_10_GTAC_30_SIC_Index2_08_CTGGTGG_AAGCACGT_S51_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_11_GTAC_31_SIC_Index2_08_TGCCCAT_AAGCACGT_S52_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_12_GTAC_32_SIC_Index2_08_AAACCTT_AAGCACGT_S53_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_13_GTAC_33_SIC_Index2_08_ACCATAC_AAGCACGT_S54_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_14_GTAC_34_SIC_Index2_08_AATACGC_AAGCACGT_S55_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_15_GTAC_35_SIC_Index2_08_CGCTACA_AAGCACGT_S56_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_16_GTAC_36_SIC_Index2_08_TGGCATA_AAGCACGT_S57_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_17_GTAC_37_SIC_Index2_08_TTTTGTC_AAGCACGT_S58_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_18_GTAC_38_SIC_Index2_08_ACCCACT_AAGCACGT_S59_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_19_GTAC_39_SIC_Index2_08_CCGGACC_AAGCACGT_S60_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_21_GTAC_41_SIC_Index2_08_TTGCCCC_AAGCACGT_S61_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_22_GTAC_42_SIC_Index2_08_ACTCCAA_AAGCACGT_S10_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_23_GTAC_43_SIC_Index2_08_TGTGCCA_AAGCACGT_S11_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_24_GTAC_44_SIC_Index2_08_AACGGAG_AAGCACGT_S62_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_25_GTAC_45_SIC_Index2_08_GATAGTT_AAGCACGT_S63_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_26_GTAC_46_SIC_Index2_08_GGTGAAT_AAGCACGT_S64_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_27_GTAC_47_SIC_Index2_08_ATGTTCT_AAGCACGT_S12_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_28_GTAC_48_SIC_Index2_08_GTAAAAA_AAGCACGT_S13_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_29_GTAC_49_SIC_Index2_08_GTCTGAT_AAGCACGT_S14_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_30_GTAC_50_SIC_Index2_08_CAATATC_AAGCACGT_S15_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_31_GTAC_51_SIC_Index2_08_CTCCCGA_AAGCACGT_S65_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_32_GTAC_52_SIC_Index2_08_GCCGTTT_AAGCACGT_S66_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_33_GTAC_53_SIC_Index2_08_TAGGTAA_AAGCACGT_S67_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_34_GTAC_54_SIC_Index2_08_TCGAGAT_AAGCACGT_S16_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_35_GTAC_55_SIC_Index2_08_CATTTAG_AAGCACGT_S17_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_36_GTAC_56_SIC_Index2_08_TCCGGGA_AAGCACGT_S68_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_37_GTAC_57_SIC_Index2_08_CGAAAGT_AAGCACGT_S18_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_38_GTAC_58_SIC_Index2_08_GCCTCCC_AAGCACGT_S69_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Small/Brent_R1_39_GTAC_59_SIC_Index2_08_AGTTATG_AAGCACGT_S70_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_Large/Brent_R1_40_GTAC_60_SIC_Index2_08_CTGCAAT_AAGCACGT_S19_R1_001.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -337,9 +337,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -370,7 +370,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,13 +687,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6FE0F8-CD5D-7147-8444-F3FCBC50A636}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="M81" sqref="M81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="86.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -731,12 +734,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -763,15 +766,15 @@
         <v>5757093</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -798,15 +801,15 @@
         <v>5437333</v>
       </c>
       <c r="L3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -833,15 +836,15 @@
         <v>5598232</v>
       </c>
       <c r="L4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -868,15 +871,15 @@
         <v>8058376</v>
       </c>
       <c r="L5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -903,15 +906,15 @@
         <v>5411350</v>
       </c>
       <c r="L6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -938,15 +941,15 @@
         <v>4239091</v>
       </c>
       <c r="L7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -973,15 +976,15 @@
         <v>5489289</v>
       </c>
       <c r="L8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>7</v>
@@ -1008,15 +1011,15 @@
         <v>6039521</v>
       </c>
       <c r="L9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>8</v>
@@ -1043,15 +1046,15 @@
         <v>4530282</v>
       </c>
       <c r="L10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>9</v>
@@ -1078,15 +1081,15 @@
         <v>5231333</v>
       </c>
       <c r="L11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -1113,15 +1116,15 @@
         <v>4951980</v>
       </c>
       <c r="L12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1148,15 +1151,15 @@
         <v>15732125</v>
       </c>
       <c r="L13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -1183,15 +1186,15 @@
         <v>6127943</v>
       </c>
       <c r="L14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>11</v>
@@ -1218,15 +1221,15 @@
         <v>4798206</v>
       </c>
       <c r="L15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>12</v>
@@ -1253,15 +1256,15 @@
         <v>5429583</v>
       </c>
       <c r="L16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C17">
         <v>13</v>
@@ -1288,15 +1291,15 @@
         <v>5059067</v>
       </c>
       <c r="L17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>14</v>
@@ -1323,15 +1326,15 @@
         <v>5422234</v>
       </c>
       <c r="L18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>15</v>
@@ -1358,15 +1361,15 @@
         <v>5697744</v>
       </c>
       <c r="L19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -1393,15 +1396,15 @@
         <v>5575061</v>
       </c>
       <c r="L20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -1428,15 +1431,15 @@
         <v>6042694</v>
       </c>
       <c r="L21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C22">
         <v>6</v>
@@ -1463,15 +1466,15 @@
         <v>5231032</v>
       </c>
       <c r="L22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C23">
         <v>7</v>
@@ -1498,15 +1501,15 @@
         <v>5247134</v>
       </c>
       <c r="L23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C24">
         <v>8</v>
@@ -1533,15 +1536,15 @@
         <v>5656633</v>
       </c>
       <c r="L24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C25">
         <v>9</v>
@@ -1568,15 +1571,15 @@
         <v>5008427</v>
       </c>
       <c r="L25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C26">
         <v>16</v>
@@ -1603,15 +1606,15 @@
         <v>5695775</v>
       </c>
       <c r="L26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C27">
         <v>17</v>
@@ -1638,15 +1641,15 @@
         <v>5170807</v>
       </c>
       <c r="L27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C28">
         <v>18</v>
@@ -1673,15 +1676,15 @@
         <v>5518056</v>
       </c>
       <c r="L28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C29">
         <v>19</v>
@@ -1708,15 +1711,15 @@
         <v>4880408</v>
       </c>
       <c r="L29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C30">
         <v>20</v>
@@ -1743,15 +1746,15 @@
         <v>5516082</v>
       </c>
       <c r="L30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C31">
         <v>21</v>
@@ -1778,15 +1781,15 @@
         <v>5080692</v>
       </c>
       <c r="L31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C32">
         <v>10</v>
@@ -1813,15 +1816,15 @@
         <v>5111900</v>
       </c>
       <c r="L32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C33">
         <v>11</v>
@@ -1848,15 +1851,15 @@
         <v>5614037</v>
       </c>
       <c r="L33" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C34">
         <v>22</v>
@@ -1883,15 +1886,15 @@
         <v>4719914</v>
       </c>
       <c r="L34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C35">
         <v>23</v>
@@ -1918,15 +1921,15 @@
         <v>4407709</v>
       </c>
       <c r="L35" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C36">
         <v>24</v>
@@ -1953,15 +1956,15 @@
         <v>6670950</v>
       </c>
       <c r="L36" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C37">
         <v>25</v>
@@ -1988,15 +1991,15 @@
         <v>5726075</v>
       </c>
       <c r="L37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C38">
         <v>26</v>
@@ -2023,15 +2026,15 @@
         <v>5445474</v>
       </c>
       <c r="L38" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C39">
         <v>12</v>
@@ -2058,15 +2061,15 @@
         <v>5470821</v>
       </c>
       <c r="L39" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C40">
         <v>13</v>
@@ -2093,15 +2096,15 @@
         <v>6858667</v>
       </c>
       <c r="L40" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C41">
         <v>14</v>
@@ -2128,15 +2131,15 @@
         <v>5519227</v>
       </c>
       <c r="L41" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2163,15 +2166,15 @@
         <v>5725861</v>
       </c>
       <c r="L42" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -2198,15 +2201,15 @@
         <v>5865767</v>
       </c>
       <c r="L43" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C44">
         <v>3</v>
@@ -2233,15 +2236,15 @@
         <v>5526637</v>
       </c>
       <c r="L44" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C45">
         <v>4</v>
@@ -2268,15 +2271,15 @@
         <v>5281850</v>
       </c>
       <c r="L45" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C46">
         <v>5</v>
@@ -2303,15 +2306,15 @@
         <v>5450802</v>
       </c>
       <c r="L46" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C47">
         <v>6</v>
@@ -2338,15 +2341,15 @@
         <v>5637404</v>
       </c>
       <c r="L47" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C48">
         <v>7</v>
@@ -2373,15 +2376,15 @@
         <v>5308217</v>
       </c>
       <c r="L48" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B49" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C49">
         <v>8</v>
@@ -2408,15 +2411,15 @@
         <v>5631729</v>
       </c>
       <c r="L49" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C50">
         <v>9</v>
@@ -2443,15 +2446,15 @@
         <v>141992</v>
       </c>
       <c r="L50" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B51" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C51">
         <v>10</v>
@@ -2478,15 +2481,15 @@
         <v>4357957</v>
       </c>
       <c r="L51" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C52">
         <v>11</v>
@@ -2513,15 +2516,15 @@
         <v>1564888</v>
       </c>
       <c r="L52" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C53">
         <v>12</v>
@@ -2548,15 +2551,15 @@
         <v>4145803</v>
       </c>
       <c r="L53" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C54">
         <v>13</v>
@@ -2583,15 +2586,15 @@
         <v>4415446</v>
       </c>
       <c r="L54" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C55">
         <v>14</v>
@@ -2618,15 +2621,15 @@
         <v>4247449</v>
       </c>
       <c r="L55" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B56" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C56">
         <v>15</v>
@@ -2653,15 +2656,15 @@
         <v>2585011</v>
       </c>
       <c r="L56" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C57">
         <v>16</v>
@@ -2688,15 +2691,15 @@
         <v>49729</v>
       </c>
       <c r="L57" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C58">
         <v>17</v>
@@ -2723,15 +2726,15 @@
         <v>649789</v>
       </c>
       <c r="L58" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B59" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C59">
         <v>18</v>
@@ -2758,15 +2761,15 @@
         <v>5877431</v>
       </c>
       <c r="L59" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B60" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C60">
         <v>19</v>
@@ -2793,15 +2796,15 @@
         <v>5399904</v>
       </c>
       <c r="L60" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B61" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C61">
         <v>20</v>
@@ -2828,15 +2831,15 @@
         <v>7464627</v>
       </c>
       <c r="L61" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B62" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C62">
         <v>21</v>
@@ -2863,15 +2866,15 @@
         <v>5871686</v>
       </c>
       <c r="L62" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B63" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C63">
         <v>22</v>
@@ -2898,15 +2901,15 @@
         <v>5740620</v>
       </c>
       <c r="L63" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B64" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C64">
         <v>23</v>
@@ -2933,15 +2936,15 @@
         <v>6390055</v>
       </c>
       <c r="L64" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B65" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C65">
         <v>24</v>
@@ -2968,15 +2971,15 @@
         <v>5375811</v>
       </c>
       <c r="L65" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B66" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C66">
         <v>25</v>
@@ -3003,15 +3006,15 @@
         <v>5335368</v>
       </c>
       <c r="L66" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B67" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C67">
         <v>26</v>
@@ -3038,15 +3041,15 @@
         <v>5419195</v>
       </c>
       <c r="L67" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B68" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C68">
         <v>27</v>
@@ -3073,15 +3076,15 @@
         <v>5480388</v>
       </c>
       <c r="L68" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B69" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C69">
         <v>28</v>
@@ -3108,15 +3111,15 @@
         <v>5218035</v>
       </c>
       <c r="L69" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B70" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C70">
         <v>29</v>
@@ -3143,15 +3146,15 @@
         <v>5220321</v>
       </c>
       <c r="L70" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B71" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C71">
         <v>30</v>
@@ -3178,15 +3181,15 @@
         <v>5109464</v>
       </c>
       <c r="L71" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B72" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C72">
         <v>31</v>
@@ -3213,15 +3216,15 @@
         <v>3007602</v>
       </c>
       <c r="L72" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B73" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C73">
         <v>32</v>
@@ -3248,15 +3251,15 @@
         <v>3214189</v>
       </c>
       <c r="L73" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B74" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C74">
         <v>33</v>
@@ -3283,15 +3286,15 @@
         <v>4798372</v>
       </c>
       <c r="L74" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B75" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C75">
         <v>34</v>
@@ -3318,15 +3321,15 @@
         <v>5465309</v>
       </c>
       <c r="L75" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B76" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C76">
         <v>35</v>
@@ -3353,15 +3356,15 @@
         <v>4919709</v>
       </c>
       <c r="L76" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B77" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C77">
         <v>36</v>
@@ -3388,15 +3391,15 @@
         <v>252945</v>
       </c>
       <c r="L77" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B78" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C78">
         <v>37</v>
@@ -3423,15 +3426,15 @@
         <v>5009360</v>
       </c>
       <c r="L78" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B79" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C79">
         <v>38</v>
@@ -3458,15 +3461,15 @@
         <v>5225180</v>
       </c>
       <c r="L79" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B80" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C80">
         <v>39</v>
@@ -3493,15 +3496,15 @@
         <v>4963817</v>
       </c>
       <c r="L80" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B81" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C81">
         <v>40</v>
@@ -3528,7 +3531,7 @@
         <v>4805012</v>
       </c>
       <c r="L81" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>